<commit_message>
Add valid Login test cases
</commit_message>
<xml_diff>
--- a/2024 Test Cases.xlsx
+++ b/2024 Test Cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\QA TESTING ESSENTIALS\GIT-Hub\Mock Test Cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01B1A8D3-0DD9-4C26-B540-75A546DC80E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29BF3103-438B-4306-B73B-D40C2BADD2B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="50910" windowHeight="21840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="50910" windowHeight="21840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="95">
   <si>
     <t>Project Name</t>
   </si>
@@ -286,6 +286,39 @@
   </si>
   <si>
     <t>An error message appears informing the user that he must enter a valid password</t>
+  </si>
+  <si>
+    <t>Login using the Facebook Button</t>
+  </si>
+  <si>
+    <t>Login using the Facebook Button with user already signed in on Facebook</t>
+  </si>
+  <si>
+    <t>Login using the Google Button</t>
+  </si>
+  <si>
+    <t>Login using the Facebook Button with user already signed in on Google</t>
+  </si>
+  <si>
+    <t>• The Sign-up process completes successfully 
+• The user is redirected on (xyz) page</t>
+  </si>
+  <si>
+    <t>• The Login process completes successfully 
+• The user is redirected on (xyz) page</t>
+  </si>
+  <si>
+    <t>Click on the Sign In button</t>
+  </si>
+  <si>
+    <t>• The login process completes successfully 
+• The user is redirected on (xyz) page</t>
+  </si>
+  <si>
+    <t>Login as a Project Owner using valid credentials</t>
+  </si>
+  <si>
+    <t>Login as an Admin using valid credentials</t>
   </si>
 </sst>
 </file>
@@ -392,7 +425,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -445,12 +478,16 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1285,11 +1322,13 @@
   </sheetPr>
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:C14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="32.140625" customWidth="1"/>
+    <col min="2" max="2" width="40.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="32.7109375" customWidth="1"/>
     <col min="4" max="4" width="16.140625" customWidth="1"/>
     <col min="5" max="5" width="17.42578125" customWidth="1"/>
@@ -1327,11 +1366,11 @@
       <c r="B2" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
     </row>
     <row r="3" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8">
@@ -1356,11 +1395,11 @@
       <c r="C4" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="26" t="s">
         <v>22</v>
       </c>
       <c r="E4" s="13"/>
-      <c r="F4" s="22" t="s">
+      <c r="F4" s="26" t="s">
         <v>23</v>
       </c>
       <c r="G4" s="14"/>
@@ -1375,9 +1414,9 @@
       <c r="C5" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="23"/>
+      <c r="D5" s="25"/>
       <c r="E5" s="13"/>
-      <c r="F5" s="23"/>
+      <c r="F5" s="25"/>
       <c r="G5" s="14"/>
     </row>
     <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.2">
@@ -1390,9 +1429,9 @@
       <c r="C6" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="23"/>
+      <c r="D6" s="25"/>
       <c r="E6" s="13"/>
-      <c r="F6" s="23"/>
+      <c r="F6" s="25"/>
       <c r="G6" s="14"/>
     </row>
     <row r="7" spans="1:8" ht="60" x14ac:dyDescent="0.2">
@@ -1405,9 +1444,9 @@
       <c r="C7" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="23"/>
+      <c r="D7" s="25"/>
       <c r="E7" s="13"/>
-      <c r="F7" s="23"/>
+      <c r="F7" s="25"/>
       <c r="G7" s="14"/>
     </row>
     <row r="8" spans="1:8" ht="90" x14ac:dyDescent="0.2">
@@ -1420,9 +1459,9 @@
       <c r="C8" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="23"/>
+      <c r="D8" s="25"/>
       <c r="E8" s="13"/>
-      <c r="F8" s="23"/>
+      <c r="F8" s="25"/>
       <c r="G8" s="14"/>
     </row>
     <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.2">
@@ -1448,11 +1487,11 @@
       <c r="C10" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="22" t="s">
+      <c r="D10" s="26" t="s">
         <v>35</v>
       </c>
       <c r="E10" s="13"/>
-      <c r="F10" s="22" t="s">
+      <c r="F10" s="26" t="s">
         <v>22</v>
       </c>
       <c r="G10" s="14"/>
@@ -1467,9 +1506,9 @@
       <c r="C11" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="23"/>
+      <c r="D11" s="25"/>
       <c r="E11" s="13"/>
-      <c r="F11" s="23"/>
+      <c r="F11" s="25"/>
       <c r="G11" s="14"/>
     </row>
     <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.2">
@@ -1482,9 +1521,9 @@
       <c r="C12" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="23"/>
+      <c r="D12" s="25"/>
       <c r="E12" s="13"/>
-      <c r="F12" s="23"/>
+      <c r="F12" s="25"/>
       <c r="G12" s="14"/>
       <c r="H12" s="17" t="s">
         <v>37</v>
@@ -1500,9 +1539,9 @@
       <c r="C13" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="23"/>
+      <c r="D13" s="25"/>
       <c r="E13" s="13"/>
-      <c r="F13" s="23"/>
+      <c r="F13" s="25"/>
       <c r="G13" s="14"/>
     </row>
     <row r="14" spans="1:8" ht="90" x14ac:dyDescent="0.2">
@@ -1515,9 +1554,9 @@
       <c r="C14" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D14" s="23"/>
+      <c r="D14" s="25"/>
       <c r="E14" s="13"/>
-      <c r="F14" s="23"/>
+      <c r="F14" s="25"/>
       <c r="G14" s="14"/>
     </row>
     <row r="15" spans="1:8" ht="15" x14ac:dyDescent="0.2">
@@ -1543,11 +1582,11 @@
       <c r="C16" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="D16" s="22" t="s">
+      <c r="D16" s="26" t="s">
         <v>42</v>
       </c>
       <c r="E16" s="13"/>
-      <c r="F16" s="22" t="s">
+      <c r="F16" s="26" t="s">
         <v>35</v>
       </c>
       <c r="G16" s="14"/>
@@ -1562,9 +1601,9 @@
       <c r="C17" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="D17" s="23"/>
+      <c r="D17" s="25"/>
       <c r="E17" s="13"/>
-      <c r="F17" s="23"/>
+      <c r="F17" s="25"/>
       <c r="G17" s="14"/>
     </row>
     <row r="18" spans="1:7" ht="90" x14ac:dyDescent="0.2">
@@ -1577,9 +1616,9 @@
       <c r="C18" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="D18" s="23"/>
+      <c r="D18" s="25"/>
       <c r="E18" s="13"/>
-      <c r="F18" s="23"/>
+      <c r="F18" s="25"/>
       <c r="G18" s="14"/>
     </row>
     <row r="19" spans="1:7" ht="45" x14ac:dyDescent="0.2">
@@ -1605,11 +1644,11 @@
       <c r="C20" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="D20" s="22" t="s">
+      <c r="D20" s="26" t="s">
         <v>22</v>
       </c>
       <c r="E20" s="13"/>
-      <c r="F20" s="22" t="s">
+      <c r="F20" s="26" t="s">
         <v>23</v>
       </c>
       <c r="G20" s="14"/>
@@ -1624,9 +1663,9 @@
       <c r="C21" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="D21" s="23"/>
+      <c r="D21" s="25"/>
       <c r="E21" s="13"/>
-      <c r="F21" s="23"/>
+      <c r="F21" s="25"/>
       <c r="G21" s="14"/>
     </row>
     <row r="22" spans="1:7" ht="15" x14ac:dyDescent="0.2">
@@ -1652,11 +1691,11 @@
       <c r="C23" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="D23" s="22" t="s">
+      <c r="D23" s="26" t="s">
         <v>51</v>
       </c>
       <c r="E23" s="13"/>
-      <c r="F23" s="22" t="s">
+      <c r="F23" s="26" t="s">
         <v>51</v>
       </c>
       <c r="G23" s="14"/>
@@ -1671,9 +1710,9 @@
       <c r="C24" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="D24" s="23"/>
+      <c r="D24" s="25"/>
       <c r="E24" s="13"/>
-      <c r="F24" s="23"/>
+      <c r="F24" s="25"/>
       <c r="G24" s="14"/>
     </row>
     <row r="25" spans="1:7" ht="90" x14ac:dyDescent="0.2">
@@ -1686,9 +1725,9 @@
       <c r="C25" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="D25" s="23"/>
+      <c r="D25" s="25"/>
       <c r="E25" s="13"/>
-      <c r="F25" s="23"/>
+      <c r="F25" s="25"/>
       <c r="G25" s="14"/>
     </row>
     <row r="26" spans="1:7" ht="45" x14ac:dyDescent="0.2">
@@ -1714,11 +1753,11 @@
       <c r="C27" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="22" t="s">
+      <c r="D27" s="26" t="s">
         <v>54</v>
       </c>
       <c r="E27" s="20"/>
-      <c r="F27" s="22" t="s">
+      <c r="F27" s="26" t="s">
         <v>54</v>
       </c>
       <c r="G27" s="14"/>
@@ -1733,9 +1772,9 @@
       <c r="C28" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="D28" s="23"/>
+      <c r="D28" s="25"/>
       <c r="E28" s="20"/>
-      <c r="F28" s="23"/>
+      <c r="F28" s="25"/>
       <c r="G28" s="14"/>
     </row>
     <row r="29" spans="1:7" ht="15" x14ac:dyDescent="0.2">
@@ -1749,11 +1788,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="D4:D8"/>
-    <mergeCell ref="F4:F8"/>
-    <mergeCell ref="D10:D14"/>
-    <mergeCell ref="F10:F14"/>
     <mergeCell ref="F16:F18"/>
     <mergeCell ref="F20:F21"/>
     <mergeCell ref="D23:D25"/>
@@ -1762,6 +1796,11 @@
     <mergeCell ref="F27:F28"/>
     <mergeCell ref="D16:D18"/>
     <mergeCell ref="D20:D21"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="D4:D8"/>
+    <mergeCell ref="F4:F8"/>
+    <mergeCell ref="D10:D14"/>
+    <mergeCell ref="F10:F14"/>
   </mergeCells>
   <conditionalFormatting sqref="D4:D8 F4:F8 D10:D14 F10:F14 D16 F16 D20 F20 D23:D25 F23:F25 D27:D28 F27:F28">
     <cfRule type="cellIs" dxfId="47" priority="1" operator="equal">
@@ -1811,7 +1850,7 @@
   </sheetPr>
   <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
@@ -1854,15 +1893,15 @@
       <c r="A2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
     </row>
     <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="8">
@@ -1885,14 +1924,14 @@
       <c r="B4" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="C4" s="25" t="s">
+      <c r="C4" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="26" t="s">
         <v>22</v>
       </c>
       <c r="E4" s="13"/>
-      <c r="F4" s="22" t="s">
+      <c r="F4" s="26" t="s">
         <v>23</v>
       </c>
       <c r="G4" s="14"/>
@@ -1905,10 +1944,10 @@
       <c r="B5" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
       <c r="E5" s="13"/>
-      <c r="F5" s="23"/>
+      <c r="F5" s="25"/>
       <c r="G5" s="14"/>
       <c r="H5" s="18"/>
     </row>
@@ -1919,10 +1958,10 @@
       <c r="B6" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
       <c r="E6" s="13"/>
-      <c r="F6" s="23"/>
+      <c r="F6" s="25"/>
       <c r="G6" s="14"/>
       <c r="H6" s="18"/>
     </row>
@@ -1947,18 +1986,18 @@
       <c r="B8" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="C8" s="25" t="s">
+      <c r="C8" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="D8" s="22" t="s">
+      <c r="D8" s="26" t="s">
         <v>35</v>
       </c>
       <c r="E8" s="13"/>
-      <c r="F8" s="22" t="s">
+      <c r="F8" s="26" t="s">
         <v>22</v>
       </c>
       <c r="G8" s="14"/>
-      <c r="H8" s="25" t="s">
+      <c r="H8" s="27" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1969,12 +2008,12 @@
       <c r="B9" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="C9" s="25"/>
-      <c r="D9" s="23"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="25"/>
       <c r="E9" s="13"/>
-      <c r="F9" s="23"/>
+      <c r="F9" s="25"/>
       <c r="G9" s="14"/>
-      <c r="H9" s="25"/>
+      <c r="H9" s="27"/>
     </row>
     <row r="10" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="11">
@@ -1983,12 +2022,12 @@
       <c r="B10" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="C10" s="25"/>
-      <c r="D10" s="23"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="25"/>
       <c r="E10" s="13"/>
-      <c r="F10" s="23"/>
+      <c r="F10" s="25"/>
       <c r="G10" s="14"/>
-      <c r="H10" s="25"/>
+      <c r="H10" s="27"/>
       <c r="I10" s="17" t="s">
         <v>37</v>
       </c>
@@ -2000,12 +2039,12 @@
       <c r="B11" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="C11" s="25"/>
-      <c r="D11" s="23"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="25"/>
       <c r="E11" s="13"/>
-      <c r="F11" s="23"/>
+      <c r="F11" s="25"/>
       <c r="G11" s="14"/>
-      <c r="H11" s="25"/>
+      <c r="H11" s="27"/>
     </row>
     <row r="12" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="15">
@@ -2028,14 +2067,14 @@
       <c r="B13" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="C13" s="25" t="s">
+      <c r="C13" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="D13" s="22" t="s">
+      <c r="D13" s="26" t="s">
         <v>42</v>
       </c>
       <c r="E13" s="13"/>
-      <c r="F13" s="22" t="s">
+      <c r="F13" s="26" t="s">
         <v>35</v>
       </c>
       <c r="G13" s="14"/>
@@ -2048,10 +2087,10 @@
       <c r="B14" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="C14" s="25"/>
-      <c r="D14" s="22"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="26"/>
       <c r="E14" s="13"/>
-      <c r="F14" s="22"/>
+      <c r="F14" s="26"/>
       <c r="G14" s="14"/>
       <c r="H14" s="18"/>
     </row>
@@ -2062,10 +2101,10 @@
       <c r="B15" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="C15" s="25"/>
-      <c r="D15" s="22"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="26"/>
       <c r="E15" s="13"/>
-      <c r="F15" s="22"/>
+      <c r="F15" s="26"/>
       <c r="G15" s="14"/>
       <c r="H15" s="18"/>
     </row>
@@ -2076,10 +2115,10 @@
       <c r="B16" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="C16" s="25"/>
-      <c r="D16" s="22"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="26"/>
       <c r="E16" s="13"/>
-      <c r="F16" s="22"/>
+      <c r="F16" s="26"/>
       <c r="G16" s="14"/>
       <c r="H16" s="18"/>
     </row>
@@ -2104,18 +2143,18 @@
       <c r="B18" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="C18" s="25" t="s">
+      <c r="C18" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="D18" s="22" t="s">
+      <c r="D18" s="26" t="s">
         <v>22</v>
       </c>
       <c r="E18" s="13"/>
-      <c r="F18" s="22" t="s">
+      <c r="F18" s="26" t="s">
         <v>23</v>
       </c>
       <c r="G18" s="14"/>
-      <c r="H18" s="25" t="s">
+      <c r="H18" s="27" t="s">
         <v>65</v>
       </c>
     </row>
@@ -2126,12 +2165,12 @@
       <c r="B19" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="C19" s="25"/>
-      <c r="D19" s="22"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="26"/>
       <c r="E19" s="13"/>
-      <c r="F19" s="22"/>
+      <c r="F19" s="26"/>
       <c r="G19" s="14"/>
-      <c r="H19" s="25"/>
+      <c r="H19" s="27"/>
     </row>
     <row r="20" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" s="11">
@@ -2140,12 +2179,12 @@
       <c r="B20" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="C20" s="25"/>
-      <c r="D20" s="22"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="26"/>
       <c r="E20" s="13"/>
-      <c r="F20" s="22"/>
+      <c r="F20" s="26"/>
       <c r="G20" s="14"/>
-      <c r="H20" s="25"/>
+      <c r="H20" s="27"/>
     </row>
     <row r="21" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" s="11">
@@ -2154,12 +2193,12 @@
       <c r="B21" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="C21" s="25"/>
-      <c r="D21" s="22"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="26"/>
       <c r="E21" s="13"/>
-      <c r="F21" s="22"/>
+      <c r="F21" s="26"/>
       <c r="G21" s="14"/>
-      <c r="H21" s="25"/>
+      <c r="H21" s="27"/>
     </row>
     <row r="22" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A22" s="8">
@@ -2182,18 +2221,18 @@
       <c r="B23" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="C23" s="25" t="s">
+      <c r="C23" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="D23" s="22" t="s">
+      <c r="D23" s="26" t="s">
         <v>51</v>
       </c>
       <c r="E23" s="13"/>
-      <c r="F23" s="22" t="s">
+      <c r="F23" s="26" t="s">
         <v>51</v>
       </c>
       <c r="G23" s="14"/>
-      <c r="H23" s="25"/>
+      <c r="H23" s="27"/>
     </row>
     <row r="24" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A24" s="11">
@@ -2202,12 +2241,12 @@
       <c r="B24" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="C24" s="25"/>
-      <c r="D24" s="22"/>
+      <c r="C24" s="27"/>
+      <c r="D24" s="26"/>
       <c r="E24" s="13"/>
-      <c r="F24" s="22"/>
+      <c r="F24" s="26"/>
       <c r="G24" s="14"/>
-      <c r="H24" s="25"/>
+      <c r="H24" s="27"/>
     </row>
     <row r="25" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A25" s="11">
@@ -2216,12 +2255,12 @@
       <c r="B25" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="C25" s="25"/>
-      <c r="D25" s="22"/>
+      <c r="C25" s="27"/>
+      <c r="D25" s="26"/>
       <c r="E25" s="13"/>
-      <c r="F25" s="22"/>
+      <c r="F25" s="26"/>
       <c r="G25" s="14"/>
-      <c r="H25" s="25"/>
+      <c r="H25" s="27"/>
     </row>
     <row r="26" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A26" s="11">
@@ -2230,12 +2269,12 @@
       <c r="B26" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="C26" s="25"/>
-      <c r="D26" s="22"/>
+      <c r="C26" s="27"/>
+      <c r="D26" s="26"/>
       <c r="E26" s="13"/>
-      <c r="F26" s="22"/>
+      <c r="F26" s="26"/>
       <c r="G26" s="14"/>
-      <c r="H26" s="25"/>
+      <c r="H26" s="27"/>
     </row>
     <row r="27" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A27" s="8">
@@ -2258,18 +2297,18 @@
       <c r="B28" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="C28" s="25" t="s">
+      <c r="C28" s="27" t="s">
         <v>84</v>
       </c>
-      <c r="D28" s="22" t="s">
+      <c r="D28" s="26" t="s">
         <v>23</v>
       </c>
       <c r="E28" s="13"/>
-      <c r="F28" s="22" t="s">
+      <c r="F28" s="26" t="s">
         <v>23</v>
       </c>
       <c r="G28" s="14"/>
-      <c r="H28" s="25" t="s">
+      <c r="H28" s="27" t="s">
         <v>80</v>
       </c>
     </row>
@@ -2280,12 +2319,12 @@
       <c r="B29" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="C29" s="25"/>
-      <c r="D29" s="22"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="26"/>
       <c r="E29" s="13"/>
-      <c r="F29" s="22"/>
+      <c r="F29" s="26"/>
       <c r="G29" s="14"/>
-      <c r="H29" s="25"/>
+      <c r="H29" s="27"/>
     </row>
     <row r="30" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" s="11">
@@ -2294,12 +2333,12 @@
       <c r="B30" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="25"/>
-      <c r="D30" s="22"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="26"/>
       <c r="E30" s="13"/>
-      <c r="F30" s="22"/>
+      <c r="F30" s="26"/>
       <c r="G30" s="14"/>
-      <c r="H30" s="25"/>
+      <c r="H30" s="27"/>
     </row>
     <row r="31" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" s="11">
@@ -2308,12 +2347,12 @@
       <c r="B31" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="25"/>
-      <c r="D31" s="22"/>
+      <c r="C31" s="27"/>
+      <c r="D31" s="26"/>
       <c r="E31" s="13"/>
-      <c r="F31" s="22"/>
+      <c r="F31" s="26"/>
       <c r="G31" s="14"/>
-      <c r="H31" s="25"/>
+      <c r="H31" s="27"/>
     </row>
     <row r="32" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A32" s="15">
@@ -2336,18 +2375,18 @@
       <c r="B33" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="C33" s="25" t="s">
+      <c r="C33" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="D33" s="22" t="s">
+      <c r="D33" s="26" t="s">
         <v>54</v>
       </c>
       <c r="E33" s="20"/>
-      <c r="F33" s="22" t="s">
+      <c r="F33" s="26" t="s">
         <v>54</v>
       </c>
       <c r="G33" s="14"/>
-      <c r="H33" s="25" t="s">
+      <c r="H33" s="27" t="s">
         <v>66</v>
       </c>
     </row>
@@ -2358,12 +2397,12 @@
       <c r="B34" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="C34" s="25"/>
-      <c r="D34" s="22"/>
+      <c r="C34" s="27"/>
+      <c r="D34" s="26"/>
       <c r="E34" s="20"/>
-      <c r="F34" s="22"/>
+      <c r="F34" s="26"/>
       <c r="G34" s="14"/>
-      <c r="H34" s="25"/>
+      <c r="H34" s="27"/>
     </row>
     <row r="35" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A35" s="15"/>
@@ -2377,21 +2416,26 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="D18:D21"/>
+    <mergeCell ref="F18:F21"/>
+    <mergeCell ref="C18:C21"/>
+    <mergeCell ref="D13:D16"/>
+    <mergeCell ref="F13:F16"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="F33:F34"/>
+    <mergeCell ref="H33:H34"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="H28:H31"/>
+    <mergeCell ref="D28:D31"/>
     <mergeCell ref="F28:F31"/>
     <mergeCell ref="C23:C26"/>
     <mergeCell ref="C28:C31"/>
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="H8:H11"/>
     <mergeCell ref="H18:H21"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="F33:F34"/>
-    <mergeCell ref="H33:H34"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="H28:H31"/>
     <mergeCell ref="D23:D26"/>
     <mergeCell ref="F23:F26"/>
     <mergeCell ref="H23:H26"/>
-    <mergeCell ref="D28:D31"/>
     <mergeCell ref="C4:C6"/>
     <mergeCell ref="D4:D6"/>
     <mergeCell ref="F4:F6"/>
@@ -2399,11 +2443,6 @@
     <mergeCell ref="F8:F11"/>
     <mergeCell ref="C8:C11"/>
     <mergeCell ref="C13:C16"/>
-    <mergeCell ref="D18:D21"/>
-    <mergeCell ref="F18:F21"/>
-    <mergeCell ref="C18:C21"/>
-    <mergeCell ref="D13:D16"/>
-    <mergeCell ref="F13:F16"/>
   </mergeCells>
   <conditionalFormatting sqref="D4:D6 F4:F6 D8:D11 F8:F11 D13 F13 D18 F18 D23 F23 D33 F33">
     <cfRule type="cellIs" dxfId="41" priority="25" operator="equal">
@@ -2466,32 +2505,32 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F28">
-    <cfRule type="cellIs" dxfId="17" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="1" operator="equal">
       <formula>"Ready to Test"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F28">
-    <cfRule type="cellIs" dxfId="16" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="2" operator="equal">
       <formula>"In Testing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F28">
-    <cfRule type="cellIs" dxfId="15" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="3" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F28">
-    <cfRule type="cellIs" dxfId="14" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="4" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F28">
-    <cfRule type="cellIs" dxfId="13" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="5" operator="equal">
       <formula>"Blocked"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F28">
-    <cfRule type="cellIs" dxfId="12" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="6" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2511,14 +2550,16 @@
     <tabColor rgb="FFFFE599"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="32.140625" customWidth="1"/>
-    <col min="3" max="3" width="32.7109375" customWidth="1"/>
+    <col min="2" max="2" width="40.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.5703125" customWidth="1"/>
     <col min="4" max="4" width="16.140625" customWidth="1"/>
     <col min="5" max="5" width="17.42578125" customWidth="1"/>
     <col min="6" max="6" width="16.140625" customWidth="1"/>
@@ -2555,343 +2596,474 @@
       <c r="B2" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-    </row>
-    <row r="3" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+    </row>
+    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A3" s="8">
         <v>1</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
+      <c r="B3" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" s="16"/>
       <c r="D3" s="10"/>
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
       <c r="G3" s="10"/>
     </row>
-    <row r="4" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A4" s="11">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="22" t="s">
+      <c r="B4" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="26" t="s">
         <v>22</v>
       </c>
       <c r="E4" s="13"/>
-      <c r="F4" s="22" t="s">
+      <c r="F4" s="26" t="s">
         <v>23</v>
       </c>
       <c r="G4" s="14"/>
     </row>
-    <row r="5" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.2">
       <c r="A5" s="11">
         <v>1.2</v>
       </c>
-      <c r="B5" s="11"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="23"/>
+      <c r="B5" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="25"/>
       <c r="E5" s="13"/>
-      <c r="F5" s="23"/>
+      <c r="F5" s="25"/>
       <c r="G5" s="14"/>
     </row>
-    <row r="6" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A6" s="11">
         <v>1.3</v>
       </c>
-      <c r="B6" s="11"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="23"/>
+      <c r="B6" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="C6" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="D6" s="25"/>
       <c r="E6" s="13"/>
-      <c r="F6" s="23"/>
+      <c r="F6" s="25"/>
       <c r="G6" s="14"/>
     </row>
-    <row r="7" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A7" s="11">
-        <v>1.4</v>
-      </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="14"/>
-    </row>
-    <row r="8" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.2">
+      <c r="A7" s="15">
+        <v>2</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="C7" s="16"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="15"/>
+    </row>
+    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A8" s="11">
-        <v>1.5</v>
-      </c>
-      <c r="B8" s="11"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="23"/>
+        <v>2.1</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="26" t="s">
+        <v>35</v>
+      </c>
       <c r="E8" s="13"/>
-      <c r="F8" s="23"/>
+      <c r="F8" s="26" t="s">
+        <v>22</v>
+      </c>
       <c r="G8" s="14"/>
     </row>
-    <row r="9" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A9" s="15">
-        <v>2</v>
-      </c>
-      <c r="B9" s="9"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="15"/>
-    </row>
-    <row r="10" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.2">
+      <c r="A9" s="11">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="26"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A10" s="11">
-        <v>2.1</v>
-      </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="22" t="s">
-        <v>35</v>
-      </c>
+        <v>2.4</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="C10" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="D10" s="26"/>
       <c r="E10" s="13"/>
-      <c r="F10" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="F10" s="26"/>
       <c r="G10" s="14"/>
     </row>
     <row r="11" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A11" s="11">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="B11" s="11"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="14"/>
+      <c r="A11" s="15">
+        <v>3</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="C11" s="16"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="15"/>
     </row>
     <row r="12" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="11">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="B12" s="11"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="23"/>
+        <v>3.1</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="26" t="s">
+        <v>42</v>
+      </c>
       <c r="E12" s="13"/>
-      <c r="F12" s="23"/>
+      <c r="F12" s="26" t="s">
+        <v>35</v>
+      </c>
       <c r="G12" s="14"/>
-      <c r="H12" s="17" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A13" s="11">
-        <v>2.4</v>
-      </c>
-      <c r="B13" s="11"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="23"/>
+        <v>3.2</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" s="25"/>
       <c r="E13" s="13"/>
-      <c r="F13" s="23"/>
+      <c r="F13" s="25"/>
       <c r="G13" s="14"/>
     </row>
-    <row r="14" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A14" s="11">
-        <v>2.5</v>
-      </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="23"/>
+        <v>3.3</v>
+      </c>
+      <c r="B14" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="D14" s="25"/>
       <c r="E14" s="13"/>
-      <c r="F14" s="23"/>
+      <c r="F14" s="25"/>
       <c r="G14" s="14"/>
     </row>
-    <row r="15" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A15" s="15">
-        <v>3</v>
-      </c>
-      <c r="B15" s="8"/>
+        <v>4</v>
+      </c>
+      <c r="B15" s="21" t="s">
+        <v>86</v>
+      </c>
       <c r="C15" s="16"/>
       <c r="D15" s="10"/>
       <c r="E15" s="15"/>
       <c r="F15" s="10"/>
       <c r="G15" s="15"/>
     </row>
-    <row r="16" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A16" s="11">
-        <v>3.1</v>
-      </c>
-      <c r="B16" s="18"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="22" t="s">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" s="13"/>
+      <c r="F16" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="E16" s="13"/>
-      <c r="F16" s="22" t="s">
-        <v>35</v>
-      </c>
       <c r="G16" s="14"/>
     </row>
-    <row r="17" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.2">
       <c r="A17" s="11">
-        <v>3.2</v>
-      </c>
-      <c r="B17" s="18"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="23"/>
+        <v>4.2</v>
+      </c>
+      <c r="B17" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="D17" s="25"/>
       <c r="E17" s="13"/>
-      <c r="F17" s="23"/>
+      <c r="F17" s="25"/>
       <c r="G17" s="14"/>
     </row>
     <row r="18" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A18" s="11">
-        <v>3.3</v>
-      </c>
-      <c r="B18" s="18"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="23"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="23"/>
-      <c r="G18" s="14"/>
+      <c r="A18" s="15">
+        <v>5</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="C18" s="16"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="15"/>
     </row>
     <row r="19" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A19" s="15">
-        <v>4</v>
-      </c>
-      <c r="B19" s="8"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="15"/>
-    </row>
-    <row r="20" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="A19" s="11">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="B19" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="D19" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="E19" s="20"/>
+      <c r="F19" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="G19" s="14"/>
+    </row>
+    <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.2">
       <c r="A20" s="11">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="B20" s="18"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="E20" s="13"/>
-      <c r="F20" s="22" t="s">
-        <v>42</v>
-      </c>
+        <v>5.2</v>
+      </c>
+      <c r="B20" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20" s="26"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="26"/>
       <c r="G20" s="14"/>
     </row>
-    <row r="21" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A21" s="11">
-        <v>4.2</v>
-      </c>
-      <c r="B21" s="18"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="23"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="23"/>
+        <v>5.3</v>
+      </c>
+      <c r="B21" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="D21" s="26"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="26"/>
       <c r="G21" s="14"/>
     </row>
-    <row r="22" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A22" s="11">
-        <v>4.3</v>
-      </c>
-      <c r="B22" s="18"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="23"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="23"/>
-      <c r="G22" s="14"/>
-    </row>
-    <row r="23" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A23" s="15">
-        <v>5</v>
-      </c>
-      <c r="B23" s="21"/>
-      <c r="C23" s="16"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="15"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="15"/>
-    </row>
-    <row r="24" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.2">
+      <c r="A22" s="15">
+        <v>6</v>
+      </c>
+      <c r="B22" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="C22" s="16"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+    </row>
+    <row r="23" spans="1:7" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A23" s="11">
+        <v>6.1</v>
+      </c>
+      <c r="B23" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="E23" s="20"/>
+      <c r="F23" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="G23" s="14"/>
+    </row>
+    <row r="24" spans="1:7" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A24" s="11">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="B24" s="18"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="22" t="s">
-        <v>54</v>
-      </c>
+        <v>6.2</v>
+      </c>
+      <c r="B24" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="C24" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="D24" s="25"/>
       <c r="E24" s="20"/>
-      <c r="F24" s="22" t="s">
-        <v>51</v>
-      </c>
+      <c r="F24" s="25"/>
       <c r="G24" s="14"/>
     </row>
-    <row r="25" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A25" s="11">
-        <v>5.2</v>
-      </c>
-      <c r="B25" s="18"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="23"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="23"/>
-      <c r="G25" s="14"/>
-    </row>
-    <row r="26" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A26" s="15"/>
-      <c r="B26" s="15"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="15"/>
-      <c r="E26" s="15"/>
-      <c r="F26" s="15"/>
-      <c r="G26" s="15"/>
+    <row r="25" spans="1:7" s="22" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A25" s="15"/>
+      <c r="B25" s="15"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="F16:F18"/>
-    <mergeCell ref="F20:F22"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="F24:F25"/>
+  <mergeCells count="13">
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="F19:F21"/>
+    <mergeCell ref="F12:F14"/>
+    <mergeCell ref="F16:F17"/>
     <mergeCell ref="B2:G2"/>
-    <mergeCell ref="D4:D8"/>
-    <mergeCell ref="F4:F8"/>
-    <mergeCell ref="D10:D14"/>
-    <mergeCell ref="F10:F14"/>
-    <mergeCell ref="D16:D18"/>
-    <mergeCell ref="D20:D22"/>
+    <mergeCell ref="D4:D6"/>
+    <mergeCell ref="F4:F6"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="F8:F10"/>
+    <mergeCell ref="D12:D14"/>
+    <mergeCell ref="D16:D17"/>
   </mergeCells>
-  <conditionalFormatting sqref="D4:D8 F4:F8 D10:D14 D16 D20:D22 D24:D25 F10:F14 F16 F20:F22 F24:F25">
+  <conditionalFormatting sqref="D12 D16:D17 D19 F12 F16:F17 F19 D4:D6 F4:F6 D8:D10 F8:F10">
+    <cfRule type="cellIs" dxfId="23" priority="19" operator="equal">
+      <formula>"Ready to Test"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D12 D16:D17 D19 F12 F16:F17 F19 D4:D6 F4:F6 D8:D10 F8:F10">
+    <cfRule type="cellIs" dxfId="22" priority="20" operator="equal">
+      <formula>"In Testing"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D12 D16:D17 D19 F12 F16:F17 F19 D4:D6 F4:F6 D8:D10 F8:F10">
+    <cfRule type="cellIs" dxfId="21" priority="21" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D12 D16:D17 D19 F12 F16:F17 F19 D4:D6 F4:F6 D8:D10 F8:F10">
+    <cfRule type="cellIs" dxfId="20" priority="22" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D12 D16:D17 D19 F12 F16:F17 F19 D4:D6 F4:F6 D8:D10 F8:F10">
+    <cfRule type="cellIs" dxfId="19" priority="23" operator="equal">
+      <formula>"Blocked"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D12 D16:D17 D19 F12 F16:F17 F19 D4:D6 F4:F6 D8:D10 F8:F10">
+    <cfRule type="cellIs" dxfId="18" priority="24" operator="equal">
+      <formula>"Skipped"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D23:D24">
+    <cfRule type="cellIs" dxfId="17" priority="7" operator="equal">
+      <formula>"Ready to Test"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D23:D24">
+    <cfRule type="cellIs" dxfId="16" priority="8" operator="equal">
+      <formula>"In Testing"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D23:D24">
+    <cfRule type="cellIs" dxfId="15" priority="9" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D23:D24">
+    <cfRule type="cellIs" dxfId="14" priority="10" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D23:D24">
+    <cfRule type="cellIs" dxfId="13" priority="11" operator="equal">
+      <formula>"Blocked"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D23:D24">
+    <cfRule type="cellIs" dxfId="12" priority="12" operator="equal">
+      <formula>"Skipped"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F23:F24">
     <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
       <formula>"Ready to Test"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D4:D8 F4:F8 D10:D14 D16 D20:D22 D24:D25 F10:F14 F16 F20:F22 F24:F25">
+  <conditionalFormatting sqref="F23:F24">
     <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
       <formula>"In Testing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D4:D8 F4:F8 D10:D14 D16 D20:D22 D24:D25 F10:F14 F16 F20:F22 F24:F25">
+  <conditionalFormatting sqref="F23:F24">
     <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D4:D8 F4:F8 D10:D14 D16 D20:D22 D24:D25 F10:F14 F16 F20:F22 F24:F25">
+  <conditionalFormatting sqref="F23:F24">
     <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D4:D8 F4:F8 D10:D14 D16 D20:D22 D24:D25 F10:F14 F16 F20:F22 F24:F25">
+  <conditionalFormatting sqref="F23:F24">
     <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
       <formula>"Blocked"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D4:D8 F4:F8 D10:D14 D16 D20:D22 D24:D25 F10:F14 F16 F20:F22 F24:F25">
+  <conditionalFormatting sqref="F23:F24">
     <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D4 F4 D10 F10 D16 F16 D20 F20 D24 F24" xr:uid="{00000000-0002-0000-0300-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D4 F4 D8 F8 D12 F12 D16 F16 D19 F19 D23 F23" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>"Ready to Test,In Testing,Pass,Fail,Blocked,Skipped"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2950,11 +3122,11 @@
       <c r="B2" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
     </row>
     <row r="3" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8">
@@ -2973,11 +3145,11 @@
       </c>
       <c r="B4" s="11"/>
       <c r="C4" s="12"/>
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="26" t="s">
         <v>22</v>
       </c>
       <c r="E4" s="13"/>
-      <c r="F4" s="22" t="s">
+      <c r="F4" s="26" t="s">
         <v>23</v>
       </c>
       <c r="G4" s="14"/>
@@ -2988,9 +3160,9 @@
       </c>
       <c r="B5" s="11"/>
       <c r="C5" s="12"/>
-      <c r="D5" s="23"/>
+      <c r="D5" s="25"/>
       <c r="E5" s="13"/>
-      <c r="F5" s="23"/>
+      <c r="F5" s="25"/>
       <c r="G5" s="14"/>
     </row>
     <row r="6" spans="1:8" ht="15" x14ac:dyDescent="0.2">
@@ -2999,9 +3171,9 @@
       </c>
       <c r="B6" s="11"/>
       <c r="C6" s="12"/>
-      <c r="D6" s="23"/>
+      <c r="D6" s="25"/>
       <c r="E6" s="13"/>
-      <c r="F6" s="23"/>
+      <c r="F6" s="25"/>
       <c r="G6" s="14"/>
     </row>
     <row r="7" spans="1:8" ht="15" x14ac:dyDescent="0.2">
@@ -3010,9 +3182,9 @@
       </c>
       <c r="B7" s="11"/>
       <c r="C7" s="12"/>
-      <c r="D7" s="23"/>
+      <c r="D7" s="25"/>
       <c r="E7" s="13"/>
-      <c r="F7" s="23"/>
+      <c r="F7" s="25"/>
       <c r="G7" s="14"/>
     </row>
     <row r="8" spans="1:8" ht="15" x14ac:dyDescent="0.2">
@@ -3021,9 +3193,9 @@
       </c>
       <c r="B8" s="11"/>
       <c r="C8" s="12"/>
-      <c r="D8" s="23"/>
+      <c r="D8" s="25"/>
       <c r="E8" s="13"/>
-      <c r="F8" s="23"/>
+      <c r="F8" s="25"/>
       <c r="G8" s="14"/>
     </row>
     <row r="9" spans="1:8" ht="15" x14ac:dyDescent="0.2">
@@ -3043,11 +3215,11 @@
       </c>
       <c r="B10" s="11"/>
       <c r="C10" s="12"/>
-      <c r="D10" s="22" t="s">
+      <c r="D10" s="26" t="s">
         <v>35</v>
       </c>
       <c r="E10" s="13"/>
-      <c r="F10" s="22" t="s">
+      <c r="F10" s="26" t="s">
         <v>22</v>
       </c>
       <c r="G10" s="14"/>
@@ -3058,9 +3230,9 @@
       </c>
       <c r="B11" s="11"/>
       <c r="C11" s="12"/>
-      <c r="D11" s="23"/>
+      <c r="D11" s="25"/>
       <c r="E11" s="13"/>
-      <c r="F11" s="23"/>
+      <c r="F11" s="25"/>
       <c r="G11" s="14"/>
     </row>
     <row r="12" spans="1:8" ht="15" x14ac:dyDescent="0.2">
@@ -3069,9 +3241,9 @@
       </c>
       <c r="B12" s="11"/>
       <c r="C12" s="12"/>
-      <c r="D12" s="23"/>
+      <c r="D12" s="25"/>
       <c r="E12" s="13"/>
-      <c r="F12" s="23"/>
+      <c r="F12" s="25"/>
       <c r="G12" s="14"/>
       <c r="H12" s="17" t="s">
         <v>37</v>
@@ -3083,9 +3255,9 @@
       </c>
       <c r="B13" s="11"/>
       <c r="C13" s="12"/>
-      <c r="D13" s="23"/>
+      <c r="D13" s="25"/>
       <c r="E13" s="13"/>
-      <c r="F13" s="23"/>
+      <c r="F13" s="25"/>
       <c r="G13" s="14"/>
     </row>
     <row r="14" spans="1:8" ht="15" x14ac:dyDescent="0.2">
@@ -3094,9 +3266,9 @@
       </c>
       <c r="B14" s="11"/>
       <c r="C14" s="12"/>
-      <c r="D14" s="23"/>
+      <c r="D14" s="25"/>
       <c r="E14" s="13"/>
-      <c r="F14" s="23"/>
+      <c r="F14" s="25"/>
       <c r="G14" s="14"/>
     </row>
     <row r="15" spans="1:8" ht="15" x14ac:dyDescent="0.2">
@@ -3116,11 +3288,11 @@
       </c>
       <c r="B16" s="18"/>
       <c r="C16" s="12"/>
-      <c r="D16" s="22" t="s">
+      <c r="D16" s="26" t="s">
         <v>42</v>
       </c>
       <c r="E16" s="13"/>
-      <c r="F16" s="22" t="s">
+      <c r="F16" s="26" t="s">
         <v>35</v>
       </c>
       <c r="G16" s="14"/>
@@ -3131,9 +3303,9 @@
       </c>
       <c r="B17" s="18"/>
       <c r="C17" s="12"/>
-      <c r="D17" s="23"/>
+      <c r="D17" s="25"/>
       <c r="E17" s="13"/>
-      <c r="F17" s="23"/>
+      <c r="F17" s="25"/>
       <c r="G17" s="14"/>
     </row>
     <row r="18" spans="1:7" ht="15" x14ac:dyDescent="0.2">
@@ -3142,9 +3314,9 @@
       </c>
       <c r="B18" s="18"/>
       <c r="C18" s="12"/>
-      <c r="D18" s="23"/>
+      <c r="D18" s="25"/>
       <c r="E18" s="13"/>
-      <c r="F18" s="23"/>
+      <c r="F18" s="25"/>
       <c r="G18" s="14"/>
     </row>
     <row r="19" spans="1:7" ht="15" x14ac:dyDescent="0.2">
@@ -3164,11 +3336,11 @@
       </c>
       <c r="B20" s="18"/>
       <c r="C20" s="12"/>
-      <c r="D20" s="22" t="s">
+      <c r="D20" s="26" t="s">
         <v>51</v>
       </c>
       <c r="E20" s="13"/>
-      <c r="F20" s="22" t="s">
+      <c r="F20" s="26" t="s">
         <v>42</v>
       </c>
       <c r="G20" s="14"/>
@@ -3179,9 +3351,9 @@
       </c>
       <c r="B21" s="18"/>
       <c r="C21" s="12"/>
-      <c r="D21" s="23"/>
+      <c r="D21" s="25"/>
       <c r="E21" s="13"/>
-      <c r="F21" s="23"/>
+      <c r="F21" s="25"/>
       <c r="G21" s="14"/>
     </row>
     <row r="22" spans="1:7" ht="15" x14ac:dyDescent="0.2">
@@ -3190,9 +3362,9 @@
       </c>
       <c r="B22" s="18"/>
       <c r="C22" s="12"/>
-      <c r="D22" s="23"/>
+      <c r="D22" s="25"/>
       <c r="E22" s="13"/>
-      <c r="F22" s="23"/>
+      <c r="F22" s="25"/>
       <c r="G22" s="14"/>
     </row>
     <row r="23" spans="1:7" ht="15" x14ac:dyDescent="0.2">
@@ -3212,11 +3384,11 @@
       </c>
       <c r="B24" s="18"/>
       <c r="C24" s="12"/>
-      <c r="D24" s="22" t="s">
+      <c r="D24" s="26" t="s">
         <v>54</v>
       </c>
       <c r="E24" s="20"/>
-      <c r="F24" s="22" t="s">
+      <c r="F24" s="26" t="s">
         <v>51</v>
       </c>
       <c r="G24" s="14"/>
@@ -3227,9 +3399,9 @@
       </c>
       <c r="B25" s="18"/>
       <c r="C25" s="12"/>
-      <c r="D25" s="23"/>
+      <c r="D25" s="25"/>
       <c r="E25" s="20"/>
-      <c r="F25" s="23"/>
+      <c r="F25" s="25"/>
       <c r="G25" s="14"/>
     </row>
     <row r="26" spans="1:7" ht="15" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Add invalid login test cases
</commit_message>
<xml_diff>
--- a/2024 Test Cases.xlsx
+++ b/2024 Test Cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\QA TESTING ESSENTIALS\GIT-Hub\Mock Test Cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29BF3103-438B-4306-B73B-D40C2BADD2B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF21CDE8-C94C-47FC-B267-F52BE09269BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="50910" windowHeight="21840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="50910" windowHeight="21840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="105">
   <si>
     <t>Project Name</t>
   </si>
@@ -319,6 +319,36 @@
   </si>
   <si>
     <t>Login as an Admin using valid credentials</t>
+  </si>
+  <si>
+    <t>Login with no username</t>
+  </si>
+  <si>
+    <t>Click on Sign In</t>
+  </si>
+  <si>
+    <t>Enter a password in the password text field</t>
+  </si>
+  <si>
+    <t>Sign-Up with invalid username</t>
+  </si>
+  <si>
+    <t>An error message appears informing the user that he must enter a valid username</t>
+  </si>
+  <si>
+    <t>Sign-Up with incorrect username</t>
+  </si>
+  <si>
+    <t>An error message appears informing the user that the username or password is incorrect</t>
+  </si>
+  <si>
+    <t>Sign-Up with incorrect password</t>
+  </si>
+  <si>
+    <t>Fill the username field with valid data</t>
+  </si>
+  <si>
+    <t>Usually not a check that is done in the Login flow</t>
   </si>
 </sst>
 </file>
@@ -425,7 +455,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -469,25 +499,23 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -495,11 +523,110 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="48">
+  <dxfs count="60">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFF7AB"/>
+          <bgColor rgb="FFFFF7AB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF9D874"/>
+          <bgColor rgb="FFF9D874"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF7AFA9"/>
+          <bgColor rgb="FFF7AFA9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC8E9C3"/>
+          <bgColor rgb="FFC8E9C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF7D7D7D"/>
+          <bgColor rgb="FF7D7D7D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE1E1E1"/>
+          <bgColor rgb="FFE1E1E1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFF7AB"/>
+          <bgColor rgb="FFFFF7AB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF9D874"/>
+          <bgColor rgb="FFF9D874"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF7AFA9"/>
+          <bgColor rgb="FFF7AFA9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC8E9C3"/>
+          <bgColor rgb="FFC8E9C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF7D7D7D"/>
+          <bgColor rgb="FF7D7D7D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE1E1E1"/>
+          <bgColor rgb="FFE1E1E1"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1018,7 +1145,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>952500</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>200025</xdr:rowOff>
@@ -1322,8 +1449,8 @@
   </sheetPr>
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C14"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B15" activeCellId="3" sqref="B26 B22 B19 B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1363,7 +1490,7 @@
       <c r="A2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="26" t="s">
         <v>18</v>
       </c>
       <c r="C2" s="25"/>
@@ -1395,11 +1522,11 @@
       <c r="C4" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="26" t="s">
+      <c r="D4" s="24" t="s">
         <v>22</v>
       </c>
       <c r="E4" s="13"/>
-      <c r="F4" s="26" t="s">
+      <c r="F4" s="24" t="s">
         <v>23</v>
       </c>
       <c r="G4" s="14"/>
@@ -1487,11 +1614,11 @@
       <c r="C10" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="26" t="s">
+      <c r="D10" s="24" t="s">
         <v>35</v>
       </c>
       <c r="E10" s="13"/>
-      <c r="F10" s="26" t="s">
+      <c r="F10" s="24" t="s">
         <v>22</v>
       </c>
       <c r="G10" s="14"/>
@@ -1563,7 +1690,7 @@
       <c r="A15" s="15">
         <v>3</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="10" t="s">
         <v>39</v>
       </c>
       <c r="C15" s="16"/>
@@ -1582,11 +1709,11 @@
       <c r="C16" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="D16" s="26" t="s">
+      <c r="D16" s="24" t="s">
         <v>42</v>
       </c>
       <c r="E16" s="13"/>
-      <c r="F16" s="26" t="s">
+      <c r="F16" s="24" t="s">
         <v>35</v>
       </c>
       <c r="G16" s="14"/>
@@ -1621,11 +1748,11 @@
       <c r="F18" s="25"/>
       <c r="G18" s="14"/>
     </row>
-    <row r="19" spans="1:7" ht="45" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.2">
       <c r="A19" s="8">
         <v>4</v>
       </c>
-      <c r="B19" s="19" t="s">
+      <c r="B19" s="16" t="s">
         <v>47</v>
       </c>
       <c r="C19" s="16"/>
@@ -1644,11 +1771,11 @@
       <c r="C20" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="D20" s="26" t="s">
+      <c r="D20" s="24" t="s">
         <v>22</v>
       </c>
       <c r="E20" s="13"/>
-      <c r="F20" s="26" t="s">
+      <c r="F20" s="24" t="s">
         <v>23</v>
       </c>
       <c r="G20" s="14"/>
@@ -1672,7 +1799,7 @@
       <c r="A22" s="8">
         <v>5</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="B22" s="10" t="s">
         <v>48</v>
       </c>
       <c r="C22" s="16"/>
@@ -1691,11 +1818,11 @@
       <c r="C23" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="D23" s="26" t="s">
+      <c r="D23" s="24" t="s">
         <v>51</v>
       </c>
       <c r="E23" s="13"/>
-      <c r="F23" s="26" t="s">
+      <c r="F23" s="24" t="s">
         <v>51</v>
       </c>
       <c r="G23" s="14"/>
@@ -1730,11 +1857,11 @@
       <c r="F25" s="25"/>
       <c r="G25" s="14"/>
     </row>
-    <row r="26" spans="1:7" ht="45" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.2">
       <c r="A26" s="8">
         <v>6</v>
       </c>
-      <c r="B26" s="19" t="s">
+      <c r="B26" s="16" t="s">
         <v>53</v>
       </c>
       <c r="C26" s="16"/>
@@ -1753,11 +1880,11 @@
       <c r="C27" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="26" t="s">
+      <c r="D27" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="E27" s="20"/>
-      <c r="F27" s="26" t="s">
+      <c r="E27" s="19"/>
+      <c r="F27" s="24" t="s">
         <v>54</v>
       </c>
       <c r="G27" s="14"/>
@@ -1773,7 +1900,7 @@
         <v>46</v>
       </c>
       <c r="D28" s="25"/>
-      <c r="E28" s="20"/>
+      <c r="E28" s="19"/>
       <c r="F28" s="25"/>
       <c r="G28" s="14"/>
     </row>
@@ -1788,6 +1915,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="D4:D8"/>
+    <mergeCell ref="F4:F8"/>
+    <mergeCell ref="D10:D14"/>
+    <mergeCell ref="F10:F14"/>
     <mergeCell ref="F16:F18"/>
     <mergeCell ref="F20:F21"/>
     <mergeCell ref="D23:D25"/>
@@ -1796,39 +1928,34 @@
     <mergeCell ref="F27:F28"/>
     <mergeCell ref="D16:D18"/>
     <mergeCell ref="D20:D21"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="D4:D8"/>
-    <mergeCell ref="F4:F8"/>
-    <mergeCell ref="D10:D14"/>
-    <mergeCell ref="F10:F14"/>
   </mergeCells>
   <conditionalFormatting sqref="D4:D8 F4:F8 D10:D14 F10:F14 D16 F16 D20 F20 D23:D25 F23:F25 D27:D28 F27:F28">
-    <cfRule type="cellIs" dxfId="47" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="1" operator="equal">
       <formula>"Ready to Test"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4:D8 F4:F8 D10:D14 F10:F14 D16 F16 D20 F20 D23:D25 F23:F25 D27:D28 F27:F28">
-    <cfRule type="cellIs" dxfId="46" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="2" operator="equal">
       <formula>"In Testing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4:D8 F4:F8 D10:D14 F10:F14 D16 F16 D20 F20 D23:D25 F23:F25 D27:D28 F27:F28">
-    <cfRule type="cellIs" dxfId="45" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="3" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4:D8 F4:F8 D10:D14 F10:F14 D16 F16 D20 F20 D23:D25 F23:F25 D27:D28 F27:F28">
-    <cfRule type="cellIs" dxfId="44" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="4" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4:D8 F4:F8 D10:D14 F10:F14 D16 F16 D20 F20 D23:D25 F23:F25 D27:D28 F27:F28">
-    <cfRule type="cellIs" dxfId="43" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="5" operator="equal">
       <formula>"Blocked"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4:D8 F4:F8 D10:D14 F10:F14 D16 F16 D20 F20 D23:D25 F23:F25 D27:D28 F27:F28">
-    <cfRule type="cellIs" dxfId="42" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="6" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1851,7 +1978,7 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+      <selection activeCell="H28" sqref="H28:H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1927,11 +2054,11 @@
       <c r="C4" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="D4" s="26" t="s">
+      <c r="D4" s="24" t="s">
         <v>22</v>
       </c>
       <c r="E4" s="13"/>
-      <c r="F4" s="26" t="s">
+      <c r="F4" s="24" t="s">
         <v>23</v>
       </c>
       <c r="G4" s="14"/>
@@ -1989,11 +2116,11 @@
       <c r="C8" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="D8" s="26" t="s">
+      <c r="D8" s="24" t="s">
         <v>35</v>
       </c>
       <c r="E8" s="13"/>
-      <c r="F8" s="26" t="s">
+      <c r="F8" s="24" t="s">
         <v>22</v>
       </c>
       <c r="G8" s="14"/>
@@ -2050,7 +2177,7 @@
       <c r="A12" s="15">
         <v>3</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="10" t="s">
         <v>76</v>
       </c>
       <c r="C12" s="16"/>
@@ -2070,11 +2197,11 @@
       <c r="C13" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="D13" s="26" t="s">
+      <c r="D13" s="24" t="s">
         <v>42</v>
       </c>
       <c r="E13" s="13"/>
-      <c r="F13" s="26" t="s">
+      <c r="F13" s="24" t="s">
         <v>35</v>
       </c>
       <c r="G13" s="14"/>
@@ -2088,9 +2215,9 @@
         <v>62</v>
       </c>
       <c r="C14" s="27"/>
-      <c r="D14" s="26"/>
+      <c r="D14" s="24"/>
       <c r="E14" s="13"/>
-      <c r="F14" s="26"/>
+      <c r="F14" s="24"/>
       <c r="G14" s="14"/>
       <c r="H14" s="18"/>
     </row>
@@ -2102,9 +2229,9 @@
         <v>58</v>
       </c>
       <c r="C15" s="27"/>
-      <c r="D15" s="26"/>
+      <c r="D15" s="24"/>
       <c r="E15" s="13"/>
-      <c r="F15" s="26"/>
+      <c r="F15" s="24"/>
       <c r="G15" s="14"/>
       <c r="H15" s="18"/>
     </row>
@@ -2116,9 +2243,9 @@
         <v>59</v>
       </c>
       <c r="C16" s="27"/>
-      <c r="D16" s="26"/>
+      <c r="D16" s="24"/>
       <c r="E16" s="13"/>
-      <c r="F16" s="26"/>
+      <c r="F16" s="24"/>
       <c r="G16" s="14"/>
       <c r="H16" s="18"/>
     </row>
@@ -2126,7 +2253,7 @@
       <c r="A17" s="8">
         <v>4</v>
       </c>
-      <c r="B17" s="19" t="s">
+      <c r="B17" s="16" t="s">
         <v>75</v>
       </c>
       <c r="C17" s="16"/>
@@ -2146,11 +2273,11 @@
       <c r="C18" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="D18" s="26" t="s">
+      <c r="D18" s="24" t="s">
         <v>22</v>
       </c>
       <c r="E18" s="13"/>
-      <c r="F18" s="26" t="s">
+      <c r="F18" s="24" t="s">
         <v>23</v>
       </c>
       <c r="G18" s="14"/>
@@ -2166,9 +2293,9 @@
         <v>63</v>
       </c>
       <c r="C19" s="27"/>
-      <c r="D19" s="26"/>
+      <c r="D19" s="24"/>
       <c r="E19" s="13"/>
-      <c r="F19" s="26"/>
+      <c r="F19" s="24"/>
       <c r="G19" s="14"/>
       <c r="H19" s="27"/>
     </row>
@@ -2180,9 +2307,9 @@
         <v>58</v>
       </c>
       <c r="C20" s="27"/>
-      <c r="D20" s="26"/>
+      <c r="D20" s="24"/>
       <c r="E20" s="13"/>
-      <c r="F20" s="26"/>
+      <c r="F20" s="24"/>
       <c r="G20" s="14"/>
       <c r="H20" s="27"/>
     </row>
@@ -2194,9 +2321,9 @@
         <v>59</v>
       </c>
       <c r="C21" s="27"/>
-      <c r="D21" s="26"/>
+      <c r="D21" s="24"/>
       <c r="E21" s="13"/>
-      <c r="F21" s="26"/>
+      <c r="F21" s="24"/>
       <c r="G21" s="14"/>
       <c r="H21" s="27"/>
     </row>
@@ -2204,7 +2331,7 @@
       <c r="A22" s="8">
         <v>5</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="B22" s="10" t="s">
         <v>78</v>
       </c>
       <c r="C22" s="16"/>
@@ -2224,11 +2351,11 @@
       <c r="C23" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="D23" s="26" t="s">
+      <c r="D23" s="24" t="s">
         <v>51</v>
       </c>
       <c r="E23" s="13"/>
-      <c r="F23" s="26" t="s">
+      <c r="F23" s="24" t="s">
         <v>51</v>
       </c>
       <c r="G23" s="14"/>
@@ -2242,9 +2369,9 @@
         <v>81</v>
       </c>
       <c r="C24" s="27"/>
-      <c r="D24" s="26"/>
+      <c r="D24" s="24"/>
       <c r="E24" s="13"/>
-      <c r="F24" s="26"/>
+      <c r="F24" s="24"/>
       <c r="G24" s="14"/>
       <c r="H24" s="27"/>
     </row>
@@ -2256,9 +2383,9 @@
         <v>58</v>
       </c>
       <c r="C25" s="27"/>
-      <c r="D25" s="26"/>
+      <c r="D25" s="24"/>
       <c r="E25" s="13"/>
-      <c r="F25" s="26"/>
+      <c r="F25" s="24"/>
       <c r="G25" s="14"/>
       <c r="H25" s="27"/>
     </row>
@@ -2270,9 +2397,9 @@
         <v>59</v>
       </c>
       <c r="C26" s="27"/>
-      <c r="D26" s="26"/>
+      <c r="D26" s="24"/>
       <c r="E26" s="13"/>
-      <c r="F26" s="26"/>
+      <c r="F26" s="24"/>
       <c r="G26" s="14"/>
       <c r="H26" s="27"/>
     </row>
@@ -2280,7 +2407,7 @@
       <c r="A27" s="8">
         <v>6</v>
       </c>
-      <c r="B27" s="19" t="s">
+      <c r="B27" s="16" t="s">
         <v>79</v>
       </c>
       <c r="C27" s="16"/>
@@ -2300,11 +2427,11 @@
       <c r="C28" s="27" t="s">
         <v>84</v>
       </c>
-      <c r="D28" s="26" t="s">
+      <c r="D28" s="24" t="s">
         <v>23</v>
       </c>
       <c r="E28" s="13"/>
-      <c r="F28" s="26" t="s">
+      <c r="F28" s="24" t="s">
         <v>23</v>
       </c>
       <c r="G28" s="14"/>
@@ -2320,9 +2447,9 @@
         <v>83</v>
       </c>
       <c r="C29" s="27"/>
-      <c r="D29" s="26"/>
+      <c r="D29" s="24"/>
       <c r="E29" s="13"/>
-      <c r="F29" s="26"/>
+      <c r="F29" s="24"/>
       <c r="G29" s="14"/>
       <c r="H29" s="27"/>
     </row>
@@ -2334,9 +2461,9 @@
         <v>58</v>
       </c>
       <c r="C30" s="27"/>
-      <c r="D30" s="26"/>
+      <c r="D30" s="24"/>
       <c r="E30" s="13"/>
-      <c r="F30" s="26"/>
+      <c r="F30" s="24"/>
       <c r="G30" s="14"/>
       <c r="H30" s="27"/>
     </row>
@@ -2348,9 +2475,9 @@
         <v>59</v>
       </c>
       <c r="C31" s="27"/>
-      <c r="D31" s="26"/>
+      <c r="D31" s="24"/>
       <c r="E31" s="13"/>
-      <c r="F31" s="26"/>
+      <c r="F31" s="24"/>
       <c r="G31" s="14"/>
       <c r="H31" s="27"/>
     </row>
@@ -2358,7 +2485,7 @@
       <c r="A32" s="15">
         <v>7</v>
       </c>
-      <c r="B32" s="21" t="s">
+      <c r="B32" s="16" t="s">
         <v>77</v>
       </c>
       <c r="C32" s="16"/>
@@ -2368,7 +2495,7 @@
       <c r="G32" s="15"/>
       <c r="H32" s="15"/>
     </row>
-    <row r="33" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A33" s="11">
         <v>7.1</v>
       </c>
@@ -2378,11 +2505,11 @@
       <c r="C33" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="D33" s="26" t="s">
+      <c r="D33" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="E33" s="20"/>
-      <c r="F33" s="26" t="s">
+      <c r="E33" s="19"/>
+      <c r="F33" s="24" t="s">
         <v>54</v>
       </c>
       <c r="G33" s="14"/>
@@ -2398,9 +2525,9 @@
         <v>68</v>
       </c>
       <c r="C34" s="27"/>
-      <c r="D34" s="26"/>
-      <c r="E34" s="20"/>
-      <c r="F34" s="26"/>
+      <c r="D34" s="24"/>
+      <c r="E34" s="19"/>
+      <c r="F34" s="24"/>
       <c r="G34" s="14"/>
       <c r="H34" s="27"/>
     </row>
@@ -2416,18 +2543,6 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="D18:D21"/>
-    <mergeCell ref="F18:F21"/>
-    <mergeCell ref="C18:C21"/>
-    <mergeCell ref="D13:D16"/>
-    <mergeCell ref="F13:F16"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="F33:F34"/>
-    <mergeCell ref="H33:H34"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="H28:H31"/>
-    <mergeCell ref="D28:D31"/>
-    <mergeCell ref="F28:F31"/>
     <mergeCell ref="C23:C26"/>
     <mergeCell ref="C28:C31"/>
     <mergeCell ref="B2:H2"/>
@@ -2443,94 +2558,106 @@
     <mergeCell ref="F8:F11"/>
     <mergeCell ref="C8:C11"/>
     <mergeCell ref="C13:C16"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="F33:F34"/>
+    <mergeCell ref="H33:H34"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="H28:H31"/>
+    <mergeCell ref="D28:D31"/>
+    <mergeCell ref="F28:F31"/>
+    <mergeCell ref="D18:D21"/>
+    <mergeCell ref="F18:F21"/>
+    <mergeCell ref="C18:C21"/>
+    <mergeCell ref="D13:D16"/>
+    <mergeCell ref="F13:F16"/>
   </mergeCells>
   <conditionalFormatting sqref="D4:D6 F4:F6 D8:D11 F8:F11 D13 F13 D18 F18 D23 F23 D33 F33">
-    <cfRule type="cellIs" dxfId="41" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="25" operator="equal">
       <formula>"Ready to Test"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4:D6 F4:F6 D8:D11 F8:F11 D13 F13 D18 F18 D23 F23 D33 F33">
-    <cfRule type="cellIs" dxfId="40" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="26" operator="equal">
       <formula>"In Testing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4:D6 F4:F6 D8:D11 F8:F11 D13 F13 D18 F18 D23 F23 D33 F33">
-    <cfRule type="cellIs" dxfId="39" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="27" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4:D6 F4:F6 D8:D11 F8:F11 D13 F13 D18 F18 D23 F23 D33 F33">
-    <cfRule type="cellIs" dxfId="38" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="28" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4:D6 F4:F6 D8:D11 F8:F11 D13 F13 D18 F18 D23 F23 D33 F33">
-    <cfRule type="cellIs" dxfId="37" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="29" operator="equal">
       <formula>"Blocked"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4:D6 F4:F6 D8:D11 F8:F11 D13 F13 D18 F18 D23 F23 D33 F33">
-    <cfRule type="cellIs" dxfId="36" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="30" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D28">
-    <cfRule type="cellIs" dxfId="35" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="7" operator="equal">
       <formula>"Ready to Test"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D28">
-    <cfRule type="cellIs" dxfId="34" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="8" operator="equal">
       <formula>"In Testing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D28">
-    <cfRule type="cellIs" dxfId="33" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="9" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D28">
-    <cfRule type="cellIs" dxfId="32" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="10" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D28">
-    <cfRule type="cellIs" dxfId="31" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="11" operator="equal">
       <formula>"Blocked"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D28">
-    <cfRule type="cellIs" dxfId="30" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="12" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F28">
-    <cfRule type="cellIs" dxfId="29" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="1" operator="equal">
       <formula>"Ready to Test"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F28">
-    <cfRule type="cellIs" dxfId="28" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="2" operator="equal">
       <formula>"In Testing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F28">
-    <cfRule type="cellIs" dxfId="27" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="3" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F28">
-    <cfRule type="cellIs" dxfId="26" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="4" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F28">
-    <cfRule type="cellIs" dxfId="25" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="5" operator="equal">
       <formula>"Blocked"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F28">
-    <cfRule type="cellIs" dxfId="24" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="6" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2552,8 +2679,8 @@
   </sheetPr>
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B22" activeCellId="3" sqref="B11 B15 B18 B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2561,9 +2688,9 @@
     <col min="2" max="2" width="40.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="44.5703125" customWidth="1"/>
     <col min="4" max="4" width="16.140625" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.140625" customWidth="1"/>
-    <col min="7" max="7" width="18.42578125" customWidth="1"/>
+    <col min="7" max="7" width="21.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.25">
@@ -2593,7 +2720,7 @@
       <c r="A2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="26" t="s">
         <v>18</v>
       </c>
       <c r="C2" s="25"/>
@@ -2602,7 +2729,7 @@
       <c r="F2" s="25"/>
       <c r="G2" s="25"/>
     </row>
-    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="8">
         <v>1</v>
       </c>
@@ -2622,14 +2749,14 @@
       <c r="B4" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="26" t="s">
+      <c r="D4" s="24" t="s">
         <v>22</v>
       </c>
       <c r="E4" s="13"/>
-      <c r="F4" s="26" t="s">
+      <c r="F4" s="24" t="s">
         <v>23</v>
       </c>
       <c r="G4" s="14"/>
@@ -2641,7 +2768,7 @@
       <c r="B5" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D5" s="25"/>
@@ -2656,7 +2783,7 @@
       <c r="B6" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="C6" s="21" t="s">
         <v>92</v>
       </c>
       <c r="D6" s="25"/>
@@ -2684,14 +2811,14 @@
       <c r="B8" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="23" t="s">
+      <c r="C8" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="26" t="s">
+      <c r="D8" s="24" t="s">
         <v>35</v>
       </c>
       <c r="E8" s="13"/>
-      <c r="F8" s="26" t="s">
+      <c r="F8" s="24" t="s">
         <v>22</v>
       </c>
       <c r="G8" s="14"/>
@@ -2703,12 +2830,12 @@
       <c r="B9" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="23" t="s">
+      <c r="C9" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="26"/>
+      <c r="D9" s="24"/>
       <c r="E9" s="13"/>
-      <c r="F9" s="26"/>
+      <c r="F9" s="24"/>
       <c r="G9" s="14"/>
       <c r="H9" s="17" t="s">
         <v>37</v>
@@ -2721,19 +2848,19 @@
       <c r="B10" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="C10" s="23" t="s">
+      <c r="C10" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="D10" s="26"/>
+      <c r="D10" s="24"/>
       <c r="E10" s="13"/>
-      <c r="F10" s="26"/>
+      <c r="F10" s="24"/>
       <c r="G10" s="14"/>
     </row>
     <row r="11" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="15">
         <v>3</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="10" t="s">
         <v>85</v>
       </c>
       <c r="C11" s="16"/>
@@ -2749,14 +2876,14 @@
       <c r="B12" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="23" t="s">
+      <c r="C12" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="D12" s="26" t="s">
+      <c r="D12" s="24" t="s">
         <v>42</v>
       </c>
       <c r="E12" s="13"/>
-      <c r="F12" s="26" t="s">
+      <c r="F12" s="24" t="s">
         <v>35</v>
       </c>
       <c r="G12" s="14"/>
@@ -2768,7 +2895,7 @@
       <c r="B13" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="C13" s="23" t="s">
+      <c r="C13" s="21" t="s">
         <v>44</v>
       </c>
       <c r="D13" s="25"/>
@@ -2783,7 +2910,7 @@
       <c r="B14" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="C14" s="23" t="s">
+      <c r="C14" s="21" t="s">
         <v>89</v>
       </c>
       <c r="D14" s="25"/>
@@ -2795,7 +2922,7 @@
       <c r="A15" s="15">
         <v>4</v>
       </c>
-      <c r="B15" s="21" t="s">
+      <c r="B15" s="16" t="s">
         <v>86</v>
       </c>
       <c r="C15" s="16"/>
@@ -2811,14 +2938,14 @@
       <c r="B16" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="23" t="s">
+      <c r="C16" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="D16" s="26" t="s">
+      <c r="D16" s="24" t="s">
         <v>51</v>
       </c>
       <c r="E16" s="13"/>
-      <c r="F16" s="26" t="s">
+      <c r="F16" s="24" t="s">
         <v>42</v>
       </c>
       <c r="G16" s="14"/>
@@ -2830,7 +2957,7 @@
       <c r="B17" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="C17" s="23" t="s">
+      <c r="C17" s="21" t="s">
         <v>90</v>
       </c>
       <c r="D17" s="25"/>
@@ -2842,7 +2969,7 @@
       <c r="A18" s="15">
         <v>5</v>
       </c>
-      <c r="B18" s="15" t="s">
+      <c r="B18" s="10" t="s">
         <v>87</v>
       </c>
       <c r="C18" s="16"/>
@@ -2858,14 +2985,14 @@
       <c r="B19" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="C19" s="23" t="s">
+      <c r="C19" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="D19" s="26" t="s">
+      <c r="D19" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="E19" s="20"/>
-      <c r="F19" s="26" t="s">
+      <c r="E19" s="19"/>
+      <c r="F19" s="24" t="s">
         <v>51</v>
       </c>
       <c r="G19" s="14"/>
@@ -2877,34 +3004,34 @@
       <c r="B20" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="23" t="s">
+      <c r="C20" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="D20" s="26"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="26"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="24"/>
       <c r="G20" s="14"/>
     </row>
-    <row r="21" spans="1:7" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A21" s="11">
         <v>5.3</v>
       </c>
       <c r="B21" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="C21" s="23" t="s">
+      <c r="C21" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="D21" s="26"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="26"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="24"/>
       <c r="G21" s="14"/>
     </row>
     <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.2">
       <c r="A22" s="15">
         <v>6</v>
       </c>
-      <c r="B22" s="21" t="s">
+      <c r="B22" s="16" t="s">
         <v>88</v>
       </c>
       <c r="C22" s="16"/>
@@ -2913,41 +3040,41 @@
       <c r="F22" s="15"/>
       <c r="G22" s="15"/>
     </row>
-    <row r="23" spans="1:7" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A23" s="11">
         <v>6.1</v>
       </c>
       <c r="B23" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="C23" s="23" t="s">
+      <c r="C23" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="D23" s="26" t="s">
+      <c r="D23" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="E23" s="20"/>
-      <c r="F23" s="26" t="s">
+      <c r="E23" s="19"/>
+      <c r="F23" s="24" t="s">
         <v>54</v>
       </c>
       <c r="G23" s="14"/>
     </row>
-    <row r="24" spans="1:7" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A24" s="11">
         <v>6.2</v>
       </c>
       <c r="B24" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="C24" s="23" t="s">
+      <c r="C24" s="21" t="s">
         <v>90</v>
       </c>
       <c r="D24" s="25"/>
-      <c r="E24" s="20"/>
+      <c r="E24" s="19"/>
       <c r="F24" s="25"/>
       <c r="G24" s="14"/>
     </row>
-    <row r="25" spans="1:7" s="22" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A25" s="15"/>
       <c r="B25" s="15"/>
       <c r="C25" s="15"/>
@@ -2958,107 +3085,107 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="D4:D6"/>
+    <mergeCell ref="F4:F6"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="F8:F10"/>
     <mergeCell ref="D23:D24"/>
     <mergeCell ref="F23:F24"/>
     <mergeCell ref="D19:D21"/>
     <mergeCell ref="F19:F21"/>
     <mergeCell ref="F12:F14"/>
     <mergeCell ref="F16:F17"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="D4:D6"/>
-    <mergeCell ref="F4:F6"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="F8:F10"/>
     <mergeCell ref="D12:D14"/>
     <mergeCell ref="D16:D17"/>
   </mergeCells>
   <conditionalFormatting sqref="D12 D16:D17 D19 F12 F16:F17 F19 D4:D6 F4:F6 D8:D10 F8:F10">
-    <cfRule type="cellIs" dxfId="23" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="19" operator="equal">
       <formula>"Ready to Test"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12 D16:D17 D19 F12 F16:F17 F19 D4:D6 F4:F6 D8:D10 F8:F10">
-    <cfRule type="cellIs" dxfId="22" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="20" operator="equal">
       <formula>"In Testing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12 D16:D17 D19 F12 F16:F17 F19 D4:D6 F4:F6 D8:D10 F8:F10">
-    <cfRule type="cellIs" dxfId="21" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="21" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12 D16:D17 D19 F12 F16:F17 F19 D4:D6 F4:F6 D8:D10 F8:F10">
-    <cfRule type="cellIs" dxfId="20" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="22" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12 D16:D17 D19 F12 F16:F17 F19 D4:D6 F4:F6 D8:D10 F8:F10">
-    <cfRule type="cellIs" dxfId="19" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="23" operator="equal">
       <formula>"Blocked"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12 D16:D17 D19 F12 F16:F17 F19 D4:D6 F4:F6 D8:D10 F8:F10">
-    <cfRule type="cellIs" dxfId="18" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="24" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D23:D24">
-    <cfRule type="cellIs" dxfId="17" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="7" operator="equal">
       <formula>"Ready to Test"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D23:D24">
-    <cfRule type="cellIs" dxfId="16" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="8" operator="equal">
       <formula>"In Testing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D23:D24">
-    <cfRule type="cellIs" dxfId="15" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="9" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D23:D24">
-    <cfRule type="cellIs" dxfId="14" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="10" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D23:D24">
-    <cfRule type="cellIs" dxfId="13" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="11" operator="equal">
       <formula>"Blocked"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D23:D24">
-    <cfRule type="cellIs" dxfId="12" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="12" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F23:F24">
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="1" operator="equal">
       <formula>"Ready to Test"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F23:F24">
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="2" operator="equal">
       <formula>"In Testing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F23:F24">
-    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="3" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F23:F24">
-    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="4" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F23:F24">
-    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="5" operator="equal">
       <formula>"Blocked"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F23:F24">
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="6" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3080,16 +3207,19 @@
   </sheetPr>
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="32.140625" customWidth="1"/>
+    <col min="2" max="2" width="47" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="32.7109375" customWidth="1"/>
     <col min="4" max="4" width="16.140625" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.140625" customWidth="1"/>
-    <col min="7" max="7" width="18.42578125" customWidth="1"/>
+    <col min="7" max="7" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.5703125" style="22" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.25">
@@ -3114,297 +3244,385 @@
       <c r="G1" s="6" t="s">
         <v>16</v>
       </c>
+      <c r="H1" s="6"/>
     </row>
     <row r="2" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-    </row>
-    <row r="3" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+    </row>
+    <row r="3" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="8">
         <v>1</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
+      <c r="B3" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="C3" s="16"/>
       <c r="D3" s="10"/>
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
       <c r="G3" s="10"/>
-    </row>
-    <row r="4" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H3" s="10"/>
+    </row>
+    <row r="4" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="11">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="26" t="s">
+      <c r="B4" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4" s="24" t="s">
         <v>22</v>
       </c>
       <c r="E4" s="13"/>
-      <c r="F4" s="26" t="s">
+      <c r="F4" s="24" t="s">
         <v>23</v>
       </c>
       <c r="G4" s="14"/>
+      <c r="H4" s="18"/>
     </row>
     <row r="5" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="11">
         <v>1.2</v>
       </c>
-      <c r="B5" s="11"/>
-      <c r="C5" s="12"/>
+      <c r="B5" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="C5" s="27"/>
       <c r="D5" s="25"/>
       <c r="E5" s="13"/>
       <c r="F5" s="25"/>
       <c r="G5" s="14"/>
+      <c r="H5" s="18"/>
     </row>
     <row r="6" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="11">
         <v>1.3</v>
       </c>
-      <c r="B6" s="11"/>
-      <c r="C6" s="12"/>
+      <c r="B6" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="C6" s="27"/>
       <c r="D6" s="25"/>
       <c r="E6" s="13"/>
       <c r="F6" s="25"/>
       <c r="G6" s="14"/>
-    </row>
-    <row r="7" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A7" s="11">
-        <v>1.4</v>
-      </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="14"/>
-    </row>
-    <row r="8" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="H6" s="18"/>
+    </row>
+    <row r="7" spans="1:8" s="22" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A7" s="15">
+        <v>2</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+    </row>
+    <row r="8" spans="1:8" s="22" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="11">
-        <v>1.5</v>
-      </c>
-      <c r="B8" s="11"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="25"/>
+        <v>2.1</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="23"/>
+      <c r="F8" s="24" t="s">
+        <v>22</v>
+      </c>
       <c r="G8" s="14"/>
-    </row>
-    <row r="9" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A9" s="15">
-        <v>2</v>
-      </c>
-      <c r="B9" s="9"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="15"/>
-    </row>
-    <row r="10" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="H8" s="29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" s="22" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A9" s="11">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="C9" s="27"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="29"/>
+    </row>
+    <row r="10" spans="1:8" s="22" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="11">
-        <v>2.1</v>
-      </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="E10" s="13"/>
-      <c r="F10" s="26" t="s">
-        <v>22</v>
-      </c>
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" s="27"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="25"/>
       <c r="G10" s="14"/>
+      <c r="H10" s="29"/>
     </row>
     <row r="11" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A11" s="11">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="B11" s="11"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="14"/>
+      <c r="A11" s="15">
+        <v>3</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="C11" s="16"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
     </row>
     <row r="12" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="11">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="B12" s="11"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="25"/>
+        <v>3.1</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="C12" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="D12" s="24" t="s">
+        <v>42</v>
+      </c>
       <c r="E12" s="13"/>
-      <c r="F12" s="25"/>
+      <c r="F12" s="24" t="s">
+        <v>35</v>
+      </c>
       <c r="G12" s="14"/>
-      <c r="H12" s="17" t="s">
-        <v>37</v>
-      </c>
+      <c r="H12" s="18"/>
     </row>
     <row r="13" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="11">
-        <v>2.4</v>
-      </c>
-      <c r="B13" s="11"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="25"/>
+        <v>3.2</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="C13" s="27"/>
+      <c r="D13" s="24"/>
       <c r="E13" s="13"/>
-      <c r="F13" s="25"/>
+      <c r="F13" s="24"/>
       <c r="G13" s="14"/>
-    </row>
-    <row r="14" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="H13" s="18"/>
+    </row>
+    <row r="14" spans="1:8" s="22" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" s="11">
-        <v>2.5</v>
-      </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="25"/>
+        <v>3.4</v>
+      </c>
+      <c r="B14" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" s="27"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="24"/>
       <c r="G14" s="14"/>
+      <c r="H14" s="18"/>
     </row>
     <row r="15" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="15">
-        <v>3</v>
-      </c>
-      <c r="B15" s="8"/>
+        <v>4</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>78</v>
+      </c>
       <c r="C15" s="16"/>
       <c r="D15" s="10"/>
       <c r="E15" s="15"/>
       <c r="F15" s="10"/>
       <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
     </row>
     <row r="16" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" s="11">
-        <v>3.1</v>
-      </c>
-      <c r="B16" s="18"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="26" t="s">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="C16" s="27" t="s">
+        <v>82</v>
+      </c>
+      <c r="D16" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" s="13"/>
+      <c r="F16" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="E16" s="13"/>
-      <c r="F16" s="26" t="s">
-        <v>35</v>
-      </c>
       <c r="G16" s="14"/>
-    </row>
-    <row r="17" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="H16" s="18"/>
+    </row>
+    <row r="17" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A17" s="11">
-        <v>3.2</v>
-      </c>
-      <c r="B17" s="18"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="25"/>
+        <v>4.2</v>
+      </c>
+      <c r="B17" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="C17" s="27"/>
+      <c r="D17" s="24"/>
       <c r="E17" s="13"/>
-      <c r="F17" s="25"/>
+      <c r="F17" s="24"/>
       <c r="G17" s="14"/>
-    </row>
-    <row r="18" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="H17" s="18"/>
+    </row>
+    <row r="18" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" s="11">
-        <v>3.3</v>
-      </c>
-      <c r="B18" s="18"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="25"/>
+        <v>4.3</v>
+      </c>
+      <c r="B18" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" s="27"/>
+      <c r="D18" s="24"/>
       <c r="E18" s="13"/>
-      <c r="F18" s="25"/>
+      <c r="F18" s="24"/>
       <c r="G18" s="14"/>
-    </row>
-    <row r="19" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="H18" s="18"/>
+    </row>
+    <row r="19" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" s="15">
-        <v>4</v>
-      </c>
-      <c r="B19" s="8"/>
+        <v>5</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>102</v>
+      </c>
       <c r="C19" s="16"/>
       <c r="D19" s="10"/>
       <c r="E19" s="15"/>
       <c r="F19" s="10"/>
       <c r="G19" s="15"/>
-    </row>
-    <row r="20" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="H19" s="15"/>
+    </row>
+    <row r="20" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="B20" s="18"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="26" t="s">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="B20" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="C20" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="D20" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="E20" s="19"/>
+      <c r="F20" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="E20" s="13"/>
-      <c r="F20" s="26" t="s">
-        <v>42</v>
-      </c>
       <c r="G20" s="14"/>
-    </row>
-    <row r="21" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="H20" s="18"/>
+    </row>
+    <row r="21" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="11">
-        <v>4.2</v>
-      </c>
-      <c r="B21" s="18"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="25"/>
+        <v>5.2</v>
+      </c>
+      <c r="B21" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="C21" s="27"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="24"/>
       <c r="G21" s="14"/>
-    </row>
-    <row r="22" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="H21" s="18"/>
+    </row>
+    <row r="22" spans="1:8" s="22" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A22" s="11">
-        <v>4.3</v>
-      </c>
-      <c r="B22" s="18"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="25"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="25"/>
+        <v>5.3</v>
+      </c>
+      <c r="B22" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="C22" s="27"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="24"/>
       <c r="G22" s="14"/>
-    </row>
-    <row r="23" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="H22" s="18"/>
+    </row>
+    <row r="23" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A23" s="15">
-        <v>5</v>
-      </c>
-      <c r="B23" s="21"/>
+        <v>6</v>
+      </c>
+      <c r="B23" s="16" t="s">
+        <v>77</v>
+      </c>
       <c r="C23" s="16"/>
-      <c r="D23" s="10"/>
+      <c r="D23" s="15"/>
       <c r="E23" s="15"/>
-      <c r="F23" s="10"/>
+      <c r="F23" s="15"/>
       <c r="G23" s="15"/>
-    </row>
-    <row r="24" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="H23" s="15"/>
+    </row>
+    <row r="24" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="11">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="B24" s="18"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="26" t="s">
+        <v>6.1</v>
+      </c>
+      <c r="B24" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="C24" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="D24" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="E24" s="20"/>
-      <c r="F24" s="26" t="s">
-        <v>51</v>
+      <c r="E24" s="19"/>
+      <c r="F24" s="24" t="s">
+        <v>54</v>
       </c>
       <c r="G24" s="14"/>
-    </row>
-    <row r="25" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="H24" s="27" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="11">
-        <v>5.2</v>
-      </c>
-      <c r="B25" s="18"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="25"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="25"/>
+        <v>6.2</v>
+      </c>
+      <c r="B25" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="C25" s="27"/>
+      <c r="D25" s="24"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="24"/>
       <c r="G25" s="14"/>
-    </row>
-    <row r="26" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="H25" s="27"/>
+    </row>
+    <row r="26" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A26" s="15"/>
       <c r="B26" s="15"/>
       <c r="C26" s="15"/>
@@ -3412,53 +3630,124 @@
       <c r="E26" s="15"/>
       <c r="F26" s="15"/>
       <c r="G26" s="15"/>
+      <c r="H26" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="21">
+    <mergeCell ref="H24:H25"/>
+    <mergeCell ref="H8:H10"/>
+    <mergeCell ref="D16:D18"/>
     <mergeCell ref="F16:F18"/>
-    <mergeCell ref="F20:F22"/>
+    <mergeCell ref="D12:D14"/>
+    <mergeCell ref="F12:F14"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="F8:F10"/>
+    <mergeCell ref="C24:C25"/>
     <mergeCell ref="D24:D25"/>
     <mergeCell ref="F24:F25"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="D4:D8"/>
-    <mergeCell ref="F4:F8"/>
-    <mergeCell ref="D10:D14"/>
-    <mergeCell ref="F10:F14"/>
-    <mergeCell ref="D16:D18"/>
     <mergeCell ref="D20:D22"/>
+    <mergeCell ref="F20:F22"/>
+    <mergeCell ref="D4:D6"/>
+    <mergeCell ref="F4:F6"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="C16:C18"/>
+    <mergeCell ref="C20:C22"/>
   </mergeCells>
-  <conditionalFormatting sqref="D4:D8 F4:F8 D10:D14 D16 D20:D22 D24:D25 F10:F14 F16 F20:F22 F24:F25">
+  <conditionalFormatting sqref="D4:D6 F4:F6 D12 D16 D20 F12 F16 F20 D8:D10 F8:F10">
+    <cfRule type="cellIs" dxfId="17" priority="19" operator="equal">
+      <formula>"Ready to Test"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D4:D6 F4:F6 D12 D16 D20 F12 F16 F20 D8:D10 F8:F10">
+    <cfRule type="cellIs" dxfId="16" priority="20" operator="equal">
+      <formula>"In Testing"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D4:D6 F4:F6 D12 D16 D20 F12 F16 F20 D8:D10 F8:F10">
+    <cfRule type="cellIs" dxfId="15" priority="21" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D4:D6 F4:F6 D12 D16 D20 F12 F16 F20 D8:D10 F8:F10">
+    <cfRule type="cellIs" dxfId="14" priority="22" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D4:D6 F4:F6 D12 D16 D20 F12 F16 F20 D8:D10 F8:F10">
+    <cfRule type="cellIs" dxfId="13" priority="23" operator="equal">
+      <formula>"Blocked"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D4:D6 F4:F6 D12 D16 D20 F12 F16 F20 D8:D10 F8:F10">
+    <cfRule type="cellIs" dxfId="12" priority="24" operator="equal">
+      <formula>"Skipped"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D24">
+    <cfRule type="cellIs" dxfId="11" priority="7" operator="equal">
+      <formula>"Ready to Test"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D24">
+    <cfRule type="cellIs" dxfId="10" priority="8" operator="equal">
+      <formula>"In Testing"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D24">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D24">
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D24">
+    <cfRule type="cellIs" dxfId="7" priority="11" operator="equal">
+      <formula>"Blocked"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D24">
+    <cfRule type="cellIs" dxfId="6" priority="12" operator="equal">
+      <formula>"Skipped"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F24">
     <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>"Ready to Test"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D4:D8 F4:F8 D10:D14 D16 D20:D22 D24:D25 F10:F14 F16 F20:F22 F24:F25">
+  <conditionalFormatting sqref="F24">
     <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>"In Testing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D4:D8 F4:F8 D10:D14 D16 D20:D22 D24:D25 F10:F14 F16 F20:F22 F24:F25">
+  <conditionalFormatting sqref="F24">
     <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D4:D8 F4:F8 D10:D14 D16 D20:D22 D24:D25 F10:F14 F16 F20:F22 F24:F25">
+  <conditionalFormatting sqref="F24">
     <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D4:D8 F4:F8 D10:D14 D16 D20:D22 D24:D25 F10:F14 F16 F20:F22 F24:F25">
+  <conditionalFormatting sqref="F24">
     <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
       <formula>"Blocked"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D4:D8 F4:F8 D10:D14 D16 D20:D22 D24:D25 F10:F14 F16 F20:F22 F24:F25">
+  <conditionalFormatting sqref="F24">
     <cfRule type="cellIs" dxfId="0" priority="6" operator="equal">
       <formula>"Skipped"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D4 F4 D10 F10 D16 F16 D20 F20 D24 F24" xr:uid="{00000000-0002-0000-0400-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D4 F4 D12 F12 D16 F16 F20 D20 D24 F24 D8 F8" xr:uid="{00000000-0002-0000-0400-000000000000}">
       <formula1>"Ready to Test,In Testing,Pass,Fail,Blocked,Skipped"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>